<commit_message>
edits for petB primer paper
</commit_message>
<xml_diff>
--- a/R_C14_DADA2/phyloseq/colours_petb.xlsx
+++ b/R_C14_DADA2/phyloseq/colours_petb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deniseong/Documents/GitHub/TAN1810_C14/R_C14_DADA2/phyloseq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094E2FAF-1B55-E241-97C2-5823A0C5132C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F824D04-DE48-F04E-839A-512C583E5F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35400" yWindow="-3140" windowWidth="25600" windowHeight="14480" activeTab="3" xr2:uid="{8B01ED10-B277-924E-A305-DA70903B797C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16000" activeTab="3" xr2:uid="{8B01ED10-B277-924E-A305-DA70903B797C}"/>
   </bookViews>
   <sheets>
     <sheet name="genus" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="99">
   <si>
     <t>genus</t>
   </si>
@@ -304,27 +304,9 @@
     <t>#000000</t>
   </si>
   <si>
-    <t>#009933</t>
-  </si>
-  <si>
-    <t>#FFCC33</t>
-  </si>
-  <si>
-    <t>#CC9933</t>
-  </si>
-  <si>
-    <t>#00CC33</t>
-  </si>
-  <si>
-    <t>#FF6666</t>
-  </si>
-  <si>
     <t>#FF3300</t>
   </si>
   <si>
-    <t>#9900CC</t>
-  </si>
-  <si>
     <t>#FFB2B2</t>
   </si>
   <si>
@@ -332,6 +314,27 @@
   </si>
   <si>
     <t>#E57E7E</t>
+  </si>
+  <si>
+    <t>#4D4D4D</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>#51A3CC</t>
+  </si>
+  <si>
+    <t>#CC5151</t>
+  </si>
+  <si>
+    <t>#A3CC51</t>
+  </si>
+  <si>
+    <t>#6B990F</t>
+  </si>
+  <si>
+    <t>#7EC3E5</t>
   </si>
 </sst>
 </file>
@@ -1036,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3510C99-2F3C-C243-9AD3-3A99BE32039E}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1073,7 +1076,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1081,7 +1084,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1089,7 +1092,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1097,7 +1100,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1105,7 +1108,7 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1217,7 +1220,7 @@
         <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1225,7 +1228,7 @@
         <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1241,7 +1244,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1265,7 +1268,7 @@
         <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1273,7 +1276,7 @@
         <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1297,7 +1300,7 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1322,6 +1325,14 @@
       </c>
       <c r="B35" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>